<commit_message>
mildly finished with ScenarioSet
</commit_message>
<xml_diff>
--- a/out/Forecast_059039.xlsx
+++ b/out/Forecast_059039.xlsx
@@ -58,10 +58,10 @@
     <t>059039</t>
   </si>
   <si>
-    <t>2024_01_17__23_52_10</t>
-  </si>
-  <si>
-    <t>2024_01_17__23_52_40</t>
+    <t>2024_01_18__16_22_52</t>
+  </si>
+  <si>
+    <t>2024_01_18__16_23_27</t>
   </si>
   <si>
     <t>Name</t>

</xml_diff>

<commit_message>
scenario html report looking great
</commit_message>
<xml_diff>
--- a/out/Forecast_059039.xlsx
+++ b/out/Forecast_059039.xlsx
@@ -58,10 +58,10 @@
     <t>059039</t>
   </si>
   <si>
-    <t>2024_01_18__16_22_52</t>
-  </si>
-  <si>
-    <t>2024_01_18__16_23_27</t>
+    <t>2024_01_22__16_52_54</t>
+  </si>
+  <si>
+    <t>2024_01_22__16_53_19</t>
   </si>
   <si>
     <t>Name</t>
@@ -1692,13 +1692,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>38.92</v>
+        <v>0.08</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>100.08</v>
       </c>
       <c r="J3">
         <v>1599.92</v>
@@ -1721,16 +1721,16 @@
         <v>45</v>
       </c>
       <c r="B4">
-        <v>1710</v>
+        <v>1520</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>160.08</v>
+        <v>120.21</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1742,19 +1742,19 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J4">
-        <v>1499.92</v>
+        <v>1399.79</v>
       </c>
       <c r="K4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>160.08</v>
+        <v>120.21</v>
       </c>
       <c r="M4">
-        <v>1710</v>
+        <v>1520</v>
       </c>
       <c r="N4" t="s">
         <v>80</v>
@@ -1765,16 +1765,16 @@
         <v>46</v>
       </c>
       <c r="B5">
-        <v>1610</v>
+        <v>1800</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D5">
-        <v>160.08</v>
+        <v>100</v>
       </c>
       <c r="E5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1786,19 +1786,19 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J5">
-        <v>1399.92</v>
+        <v>1500</v>
       </c>
       <c r="K5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L5">
-        <v>160.08</v>
+        <v>200</v>
       </c>
       <c r="M5">
-        <v>1610</v>
+        <v>1800</v>
       </c>
       <c r="N5" t="s">
         <v>81</v>
@@ -1809,16 +1809,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1610</v>
+        <v>1800</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D6">
-        <v>160.08</v>
+        <v>100</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1833,16 +1833,16 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1399.92</v>
+        <v>1500</v>
       </c>
       <c r="K6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L6">
-        <v>160.08</v>
+        <v>200</v>
       </c>
       <c r="M6">
-        <v>1610</v>
+        <v>1800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
approx forecast now aggregates items, rounded min payment values in memo, and made milestone plots into bar plots
</commit_message>
<xml_diff>
--- a/out/Forecast_059039.xlsx
+++ b/out/Forecast_059039.xlsx
@@ -58,10 +58,10 @@
     <t>059039</t>
   </si>
   <si>
-    <t>2024_01_22__16_52_54</t>
-  </si>
-  <si>
-    <t>2024_01_22__16_53_19</t>
+    <t>2024_01_28__19_21_43</t>
+  </si>
+  <si>
+    <t>2024_01_28__19_22_07</t>
   </si>
   <si>
     <t>Name</t>

</xml_diff>